<commit_message>
- moved over voltage protection diode to forward of ideal diode and duplicated it for the other non-USB input channel - updated BOM
</commit_message>
<xml_diff>
--- a/beba.xlsx
+++ b/beba.xlsx
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
- optimization of BOM: replaced MCP73871's VPCC 50k resistor with 49.9k
</commit_message>
<xml_diff>
--- a/beba.xlsx
+++ b/beba.xlsx
@@ -15,14 +15,14 @@
     <sheet name="beba" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">beba!$A$1:$G$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">beba!$A$1:$G$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>Qty</t>
   </si>
@@ -96,9 +96,6 @@
     <t>TPS630701-1:C13, TPS630701-1:C14, TPS630701-1:C15</t>
   </si>
   <si>
-    <t>MCP73871-1:R4</t>
-  </si>
-  <si>
     <t>C-POL</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>Z-Diode</t>
   </si>
   <si>
-    <t>50k</t>
-  </si>
-  <si>
     <t>SMD5</t>
   </si>
   <si>
@@ -340,9 +334,6 @@
   </si>
   <si>
     <t xml:space="preserve">78-SQ2310ES-T1_BE3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">71-PNM0805E5002BST1 </t>
   </si>
 </sst>
 </file>
@@ -1177,10 +1168,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,15 +1206,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1237,7 +1229,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1254,13 +1246,13 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1277,21 +1269,21 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1300,13 +1292,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1329,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1352,15 +1344,15 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1375,58 +1367,58 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>75</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>77</v>
       </c>
-      <c r="F9" t="s">
-        <v>78</v>
-      </c>
       <c r="G9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -1435,243 +1427,240 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>3</v>
-      </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
       <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
         <v>39</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
       </c>
       <c r="G16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
         <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>3</v>
-      </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" t="s">
         <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1679,63 +1668,49 @@
         <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>98</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23">
+        <v>1616</v>
+      </c>
+      <c r="E23" t="s">
         <v>96</v>
       </c>
-      <c r="E23" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" t="s">
-        <v>100</v>
-      </c>
       <c r="G23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24">
-        <v>1616</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G24"/>
+  <autoFilter ref="A1:G23">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="RESISTOR, European symbol"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- exchanged passives (capacitors with higher voltage, resistors with higher power rating), updated BOM
</commit_message>
<xml_diff>
--- a/beba.xlsx
+++ b/beba.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t>Qty</t>
   </si>
@@ -165,36 +165,6 @@
     <t>XFL4020-152MEC</t>
   </si>
   <si>
-    <t>4700uF / 10V</t>
-  </si>
-  <si>
-    <t>81-GRM21BR70J106KA3L</t>
-  </si>
-  <si>
-    <t>603-CC805KRX7R9BB104</t>
-  </si>
-  <si>
-    <t>581-0805ZD226MAT4A</t>
-  </si>
-  <si>
-    <t>755-KTR10EZPJ102</t>
-  </si>
-  <si>
-    <t>303-0805W8F4992T5E</t>
-  </si>
-  <si>
-    <t>303-0805W8J0753T5E</t>
-  </si>
-  <si>
-    <t>603-RC0805JR-07150KL</t>
-  </si>
-  <si>
-    <t>303-HP05W3F1002T5E</t>
-  </si>
-  <si>
-    <t>303-HP05W3J0104T5E</t>
-  </si>
-  <si>
     <t>859-LTST-C230KGKT</t>
   </si>
   <si>
@@ -207,42 +177,24 @@
     <t>595-TPS630701RNMT</t>
   </si>
   <si>
-    <t>647-UVZ1E472MHD</t>
-  </si>
-  <si>
     <t>SQ2310ES-T1_BE3</t>
   </si>
   <si>
     <t>579-MCP73871T2CCIML</t>
   </si>
   <si>
-    <t>595-LM74670QDGKTQ1</t>
-  </si>
-  <si>
     <t>994-XFL4020-152MEC</t>
   </si>
   <si>
-    <t>NXFT15XH103FEAB045</t>
-  </si>
-  <si>
-    <t>0.1uF / 50V</t>
-  </si>
-  <si>
     <t>MCP73871-1:R5, MCP73871-1:R8, TPS630701-1:R6</t>
   </si>
   <si>
     <t>TPS630701-1:R1</t>
   </si>
   <si>
-    <t>10uF / 6.3V</t>
-  </si>
-  <si>
     <t>MCP73871-1:C1, MCP73871-1:C2, MCP73871-1:C3, TPS630701-1:C8, TPS630701-1:C9, TPS630701-1:C10, TPS630701-1:C12</t>
   </si>
   <si>
-    <t>22u / 10V</t>
-  </si>
-  <si>
     <t>3SMBJ5921B-TP</t>
   </si>
   <si>
@@ -255,18 +207,12 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Z-Diode</t>
-  </si>
-  <si>
     <t>SMD5</t>
   </si>
   <si>
     <t>SMD2,54-5,08</t>
   </si>
   <si>
-    <t>SMD PAD</t>
-  </si>
-  <si>
     <t>MUSBR-05-F-O-B-SM-A</t>
   </si>
   <si>
@@ -318,22 +264,88 @@
     <t>USB - mini B USB 2.0 Receptacle</t>
   </si>
   <si>
-    <t>USB-A (USB TYPE-A) USB 2.0 Receptacle</t>
-  </si>
-  <si>
     <t>mouser part no.</t>
   </si>
   <si>
-    <t xml:space="preserve">833-3SMBJ5921B-TP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">200-MUSBR05FOBSMA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">200-USBASSBSM2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">78-SQ2310ES-T1_BE3 </t>
+    <t>NTC Thermistor</t>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+  </si>
+  <si>
+    <t>IC, Ideal Diode Controller</t>
+  </si>
+  <si>
+    <t>IC, Switching Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Fixed Inductor 1.5uH</t>
+  </si>
+  <si>
+    <t>USB-A USB 2.0 Receptacle</t>
+  </si>
+  <si>
+    <t>81-KRM21FR61E226MF1L</t>
+  </si>
+  <si>
+    <t>22u / 25V</t>
+  </si>
+  <si>
+    <t>81-GRM21BR61E106MA3L</t>
+  </si>
+  <si>
+    <t>10uF / 25V</t>
+  </si>
+  <si>
+    <t>81-GCM21BR71E104KA7L</t>
+  </si>
+  <si>
+    <t>0.1uF / 25V</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F1001V</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F1002V</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F4992V</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F1003V</t>
+  </si>
+  <si>
+    <t>667-ERJ-P06F1503V</t>
+  </si>
+  <si>
+    <t>667-ERJ-PB6D7502V</t>
+  </si>
+  <si>
+    <t>833-3SMBJ5921B-TP</t>
+  </si>
+  <si>
+    <t>200-MUSBR05FOBSMA</t>
+  </si>
+  <si>
+    <t>200-USBASSBSM2</t>
+  </si>
+  <si>
+    <t>78-SQ2310ES-T1_BE3</t>
+  </si>
+  <si>
+    <t>MCP73871-2CC</t>
+  </si>
+  <si>
+    <t>81-NXFT15XH103FEAB45</t>
+  </si>
+  <si>
+    <t>595-LM74670QDGKRQ1</t>
+  </si>
+  <si>
+    <t>647-UFW1C682MHD</t>
+  </si>
+  <si>
+    <t>6800uF / 16V</t>
   </si>
 </sst>
 </file>
@@ -1168,11 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,15 +1217,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1229,7 +1240,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1246,13 +1257,13 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,21 +1280,21 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1292,13 +1303,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1321,7 +1332,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1344,15 +1355,15 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1367,38 +1378,38 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -1409,8 +1420,11 @@
       <c r="E10" t="s">
         <v>26</v>
       </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1433,15 +1447,15 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1456,7 +1470,7 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1479,10 +1493,10 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1498,11 +1512,14 @@
       <c r="E14" t="s">
         <v>34</v>
       </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
       <c r="G14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1522,10 +1539,10 @@
         <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1545,10 +1562,10 @@
         <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1568,84 +1585,84 @@
         <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -1654,36 +1671,39 @@
         <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1697,20 +1717,17 @@
         <v>1616</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G23">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="RESISTOR, European symbol"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>